<commit_message>
Some bugfixes in calculation routines.
</commit_message>
<xml_diff>
--- a/input/data/data.xlsx
+++ b/input/data/data.xlsx
@@ -7227,11 +7227,11 @@
   </sheetPr>
   <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D37" activeCellId="0" sqref="D37"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K14" activeCellId="0" sqref="K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.72"/>
@@ -8323,7 +8323,7 @@
       <selection pane="topLeft" activeCell="D32" activeCellId="0" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.23"/>
@@ -8572,7 +8572,7 @@
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -8640,7 +8640,7 @@
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="13.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.69"/>
@@ -8722,7 +8722,7 @@
       <selection pane="topLeft" activeCell="D37" activeCellId="0" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.16"/>
@@ -8812,7 +8812,7 @@
       <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.83"/>
   </cols>
@@ -8908,7 +8908,7 @@
       <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.52"/>
@@ -15263,7 +15263,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="18"/>

</xml_diff>

<commit_message>
Bugfix in cost calculation.
</commit_message>
<xml_diff>
--- a/input/data/data.xlsx
+++ b/input/data/data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="technology_data" sheetId="1" state="visible" r:id="rId2"/>
@@ -7224,11 +7224,11 @@
   </sheetPr>
   <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B38" activeCellId="0" sqref="B38"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B37" activeCellId="0" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.76953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.72"/>
@@ -8201,7 +8201,7 @@
         <v>11</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>45</v>
@@ -8232,7 +8232,7 @@
         <v>11</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>45</v>
@@ -8316,11 +8316,11 @@
   </sheetPr>
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D32" activeCellId="0" sqref="D32"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.23"/>
@@ -8405,7 +8405,7 @@
         <v>54</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>2025</v>
@@ -8569,7 +8569,7 @@
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -8637,7 +8637,7 @@
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="13.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.69"/>
@@ -8719,7 +8719,7 @@
       <selection pane="topLeft" activeCell="D37" activeCellId="0" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.76953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.16"/>
@@ -8809,7 +8809,7 @@
       <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.76953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.83"/>
   </cols>
@@ -8905,7 +8905,7 @@
       <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.76953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.52"/>
@@ -15260,7 +15260,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.76953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="18"/>

</xml_diff>

<commit_message>
Minor updates to data format and calculations.
* Added column for value uncertainty.
* Added unit of output for processes.
* Duplicate entries are now aggregated.
</commit_message>
<xml_diff>
--- a/input/data/data.xlsx
+++ b/input/data/data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="technology_data" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,8 +14,8 @@
     <sheet name="routes" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">technology_data!$A$1:$K$37</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">technology_data!$A:$K</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">technology_data!$A:$L</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">technology_data!$A$1:$L$37</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="93">
   <si>
     <t xml:space="preserve">process_group</t>
   </si>
@@ -44,18 +44,21 @@
     <t xml:space="preserve">subcomponent</t>
   </si>
   <si>
+    <t xml:space="preserve">mode</t>
+  </si>
+  <si>
     <t xml:space="preserve">unit</t>
   </si>
   <si>
     <t xml:space="preserve">val</t>
   </si>
   <si>
+    <t xml:space="preserve">val_uncertainty</t>
+  </si>
+  <si>
     <t xml:space="preserve">val_year</t>
   </si>
   <si>
-    <t xml:space="preserve">mode</t>
-  </si>
-  <si>
     <t xml:space="preserve">source</t>
   </si>
   <si>
@@ -251,7 +254,13 @@
     <t xml:space="preserve">Electrolysis</t>
   </si>
   <si>
+    <t xml:space="preserve">MWh (LHV)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Direct reduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t</t>
   </si>
   <si>
     <t xml:space="preserve">Electric-arc furnace</t>
@@ -539,17 +548,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="C1:K37" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
-  <tableColumns count="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="C1:L37" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <tableColumns count="10">
     <tableColumn id="1" name="type"/>
     <tableColumn id="2" name="component"/>
     <tableColumn id="3" name="subcomponent"/>
-    <tableColumn id="4" name="unit"/>
-    <tableColumn id="5" name="val"/>
-    <tableColumn id="6" name="val_year"/>
-    <tableColumn id="7" name="mode"/>
-    <tableColumn id="8" name="source"/>
-    <tableColumn id="9" name="comment"/>
+    <tableColumn id="4" name="mode"/>
+    <tableColumn id="5" name="unit"/>
+    <tableColumn id="6" name="val"/>
+    <tableColumn id="7" name="val_uncertainty"/>
+    <tableColumn id="8" name="val_year"/>
+    <tableColumn id="9" name="source"/>
+    <tableColumn id="10" name="comment"/>
   </tableColumns>
 </table>
 </file>
@@ -560,24 +570,26 @@
     <tabColor rgb="FFDEEBF7"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K1048576"/>
+  <dimension ref="A1:L1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J41" activeCellId="0" sqref="J41"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.82421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="24.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="17.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="12.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="3" width="5.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="9.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="17.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="9.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="9.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="17.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="12.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="3" width="9.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="3" width="5.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="17.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="9.81"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -599,10 +611,10 @@
       <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="4" t="s">
@@ -614,1472 +626,1516 @@
       <c r="K1" s="4" t="s">
         <v>10</v>
       </c>
+      <c r="L1" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="2" t="n">
+      <c r="G2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="2" t="n">
         <v>106</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>15</v>
+      <c r="K2" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="2" t="n">
+        <v>64</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="2" t="n">
-        <v>64</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
-      <c r="F4" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="10" t="n">
+      <c r="F4" s="7"/>
+      <c r="G4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="10" t="n">
         <v>230</v>
       </c>
-      <c r="H4" s="11" t="n">
+      <c r="I4" s="11"/>
+      <c r="J4" s="11" t="n">
         <v>2025</v>
       </c>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="K4" s="7"/>
+      <c r="K4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L4" s="7"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
-      <c r="F5" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="10" t="n">
+      <c r="F5" s="7"/>
+      <c r="G5" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="10" t="n">
         <v>200</v>
       </c>
-      <c r="H5" s="12" t="n">
+      <c r="I5" s="12"/>
+      <c r="J5" s="12" t="n">
         <v>2050</v>
       </c>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="K5" s="7"/>
+      <c r="K5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="L5" s="7"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
-      <c r="F6" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" s="10" t="n">
+      <c r="F6" s="7"/>
+      <c r="G6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="10" t="n">
         <v>184</v>
       </c>
-      <c r="H6" s="11"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="K6" s="7"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L6" s="7"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
-      <c r="F7" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7" s="10" t="n">
+      <c r="F7" s="7"/>
+      <c r="G7" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" s="10" t="n">
         <v>800000</v>
       </c>
-      <c r="H7" s="11" t="n">
+      <c r="I7" s="11"/>
+      <c r="J7" s="11" t="n">
         <v>2025</v>
       </c>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="K7" s="7"/>
+      <c r="K7" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="L7" s="7"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
-      <c r="F8" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G8" s="10" t="n">
+      <c r="F8" s="7"/>
+      <c r="G8" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" s="10" t="n">
         <v>300000</v>
       </c>
-      <c r="H8" s="12" t="n">
+      <c r="I8" s="12"/>
+      <c r="J8" s="12" t="n">
         <v>2050</v>
       </c>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="K8" s="7"/>
+      <c r="K8" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="L8" s="7"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F9" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="G9" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="G9" s="2" t="n">
+      <c r="H9" s="2" t="n">
         <v>0.17</v>
       </c>
-      <c r="J9" s="1" t="s">
-        <v>15</v>
+      <c r="K9" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F10" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="G10" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="G10" s="2" t="n">
+      <c r="H10" s="2" t="n">
         <v>0.4</v>
       </c>
-      <c r="J10" s="1" t="s">
-        <v>15</v>
+      <c r="K10" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G11" s="2" t="n">
+      <c r="G11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H11" s="2" t="n">
         <v>0.17</v>
       </c>
-      <c r="J11" s="1" t="s">
-        <v>15</v>
+      <c r="K11" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D12" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="9"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="9"/>
-      <c r="F12" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="G12" s="10" t="n">
+      <c r="H12" s="10" t="n">
         <v>0.329</v>
       </c>
-      <c r="H12" s="11"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K12" s="7"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="L12" s="7"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E13" s="9"/>
-      <c r="F13" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="G13" s="10" t="n">
+      <c r="F13" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H13" s="10" t="n">
         <v>1.69983</v>
       </c>
-      <c r="H13" s="11"/>
-      <c r="I13" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="J13" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="K13" s="7"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L13" s="7"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E14" s="9"/>
-      <c r="F14" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="G14" s="10" t="n">
+      <c r="F14" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H14" s="10" t="n">
         <v>0.5</v>
       </c>
-      <c r="H14" s="11"/>
-      <c r="I14" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="J14" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K14" s="7"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="L14" s="7"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E15" s="9"/>
-      <c r="F15" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="G15" s="10" t="n">
+      <c r="F15" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H15" s="10" t="n">
         <v>2.79</v>
       </c>
-      <c r="H15" s="11"/>
-      <c r="I15" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="J15" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K15" s="7"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="L15" s="7"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D16" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G16" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E16" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="G16" s="10" t="n">
+      <c r="H16" s="10" t="n">
         <v>0.753</v>
       </c>
-      <c r="H16" s="11"/>
-      <c r="I16" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="J16" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K16" s="7"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="L16" s="7"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D17" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G17" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E17" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="G17" s="10" t="n">
+      <c r="H17" s="10" t="n">
         <v>0.667</v>
       </c>
-      <c r="H17" s="11"/>
-      <c r="I17" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="J17" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K17" s="7"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="L17" s="7"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D18" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="F18" s="7"/>
+      <c r="G18" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E18" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="G18" s="10" t="n">
+      <c r="H18" s="10" t="n">
         <v>0.159</v>
       </c>
-      <c r="H18" s="11"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K18" s="7"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="L18" s="7"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C19" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E19" s="9"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="H19" s="10" t="n">
+        <v>1.47</v>
+      </c>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12" t="n">
+        <v>2025</v>
+      </c>
+      <c r="K19" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D19" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E19" s="9"/>
-      <c r="F19" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G19" s="10" t="n">
-        <v>1.47</v>
-      </c>
-      <c r="H19" s="12" t="n">
-        <v>2025</v>
-      </c>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E20" s="9"/>
-      <c r="F20" s="8" t="n">
+      <c r="F20" s="7"/>
+      <c r="G20" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="G20" s="10" t="n">
+      <c r="H20" s="10" t="n">
         <v>1.33</v>
       </c>
-      <c r="H20" s="12" t="n">
+      <c r="I20" s="12"/>
+      <c r="J20" s="12" t="n">
         <v>2050</v>
       </c>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
       <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G21" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H21" s="2" t="n">
         <v>110</v>
       </c>
-      <c r="J21" s="1" t="s">
-        <v>15</v>
+      <c r="K21" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G22" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H22" s="2" t="n">
         <v>143</v>
       </c>
-      <c r="J22" s="1" t="s">
-        <v>15</v>
+      <c r="K22" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F23" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="G23" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="G23" s="2" t="n">
+      <c r="H23" s="2" t="n">
         <v>0.278</v>
       </c>
-      <c r="J23" s="1" t="s">
-        <v>15</v>
+      <c r="K23" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F24" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="G24" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="G24" s="2" t="n">
+      <c r="H24" s="2" t="n">
         <v>1.5</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B25" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E25" s="9"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="H25" s="10" t="n">
+        <v>0.011</v>
+      </c>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C25" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="E25" s="9"/>
-      <c r="F25" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G25" s="10" t="n">
-        <v>0.011</v>
-      </c>
-      <c r="H25" s="11"/>
-      <c r="I25" s="7"/>
-      <c r="J25" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K25" s="7"/>
+      <c r="L25" s="7"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G26" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H26" s="2" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="K26" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F26" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="G26" s="2" t="n">
-        <v>0.18</v>
-      </c>
-      <c r="J26" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B27" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E27" s="9"/>
+      <c r="F27" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G27" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="H27" s="10" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="I27" s="11"/>
+      <c r="J27" s="11"/>
+      <c r="K27" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C27" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="E27" s="9"/>
-      <c r="F27" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G27" s="10" t="n">
-        <v>0.85</v>
-      </c>
-      <c r="H27" s="11"/>
-      <c r="I27" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="J27" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K27" s="7"/>
+      <c r="L27" s="7"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B28" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E28" s="9"/>
+      <c r="F28" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G28" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="H28" s="10" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="I28" s="11"/>
+      <c r="J28" s="11"/>
+      <c r="K28" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C28" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="E28" s="9"/>
-      <c r="F28" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G28" s="10" t="n">
-        <v>0.35</v>
-      </c>
-      <c r="H28" s="11"/>
-      <c r="I28" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="J28" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K28" s="7"/>
+      <c r="L28" s="7"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B29" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E29" s="9"/>
+      <c r="F29" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G29" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="H29" s="10" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="I29" s="11"/>
+      <c r="J29" s="11"/>
+      <c r="K29" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C29" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="E29" s="9"/>
-      <c r="F29" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G29" s="10" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="H29" s="11"/>
-      <c r="I29" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="J29" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K29" s="7"/>
+      <c r="L29" s="7"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B30" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E30" s="9"/>
+      <c r="F30" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G30" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="H30" s="10" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I30" s="11"/>
+      <c r="J30" s="11"/>
+      <c r="K30" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C30" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D30" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="E30" s="9"/>
-      <c r="F30" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G30" s="10" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="H30" s="11"/>
-      <c r="I30" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="J30" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K30" s="7"/>
+      <c r="L30" s="7"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E31" s="9"/>
-      <c r="F31" s="8" t="n">
+      <c r="F31" s="7"/>
+      <c r="G31" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="G31" s="10" t="n">
+      <c r="H31" s="10" t="n">
         <v>1.504</v>
       </c>
-      <c r="H31" s="11"/>
-      <c r="I31" s="7"/>
-      <c r="J31" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K31" s="7"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="11"/>
+      <c r="K31" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="L31" s="7"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E32" s="9"/>
-      <c r="F32" s="8" t="n">
+      <c r="F32" s="7"/>
+      <c r="G32" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="G32" s="10" t="n">
+      <c r="H32" s="10" t="n">
         <v>0.011</v>
       </c>
-      <c r="H32" s="11"/>
-      <c r="I32" s="7"/>
-      <c r="J32" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K32" s="7"/>
+      <c r="I32" s="11"/>
+      <c r="J32" s="11"/>
+      <c r="K32" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="L32" s="7"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E33" s="9"/>
-      <c r="F33" s="8" t="n">
+      <c r="F33" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G33" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="G33" s="10" t="n">
+      <c r="H33" s="10" t="n">
         <v>0.85</v>
       </c>
-      <c r="H33" s="11"/>
-      <c r="I33" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="J33" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K33" s="7"/>
+      <c r="I33" s="11"/>
+      <c r="J33" s="11"/>
+      <c r="K33" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="L33" s="7"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E34" s="9"/>
-      <c r="F34" s="8" t="n">
+      <c r="F34" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G34" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="G34" s="10" t="n">
+      <c r="H34" s="10" t="n">
         <v>0.35</v>
       </c>
-      <c r="H34" s="11"/>
-      <c r="I34" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="J34" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K34" s="7"/>
+      <c r="I34" s="11"/>
+      <c r="J34" s="11"/>
+      <c r="K34" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="L34" s="7"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E35" s="9"/>
-      <c r="F35" s="8" t="n">
+      <c r="F35" s="7"/>
+      <c r="G35" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="G35" s="10" t="n">
+      <c r="H35" s="10" t="n">
         <v>0.002</v>
       </c>
-      <c r="H35" s="11"/>
-      <c r="I35" s="7"/>
-      <c r="J35" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K35" s="7"/>
+      <c r="I35" s="11"/>
+      <c r="J35" s="11"/>
+      <c r="K35" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="L35" s="7"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E36" s="9"/>
-      <c r="F36" s="8" t="n">
+      <c r="F36" s="7"/>
+      <c r="G36" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="G36" s="10" t="n">
+      <c r="H36" s="10" t="n">
         <v>0.05</v>
       </c>
-      <c r="H36" s="11"/>
-      <c r="I36" s="7"/>
-      <c r="J36" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K36" s="7"/>
+      <c r="I36" s="11"/>
+      <c r="J36" s="11"/>
+      <c r="K36" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="L36" s="7"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E37" s="9"/>
-      <c r="F37" s="8" t="n">
+      <c r="F37" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G37" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="G37" s="10" t="n">
+      <c r="H37" s="10" t="n">
         <v>0.1</v>
       </c>
-      <c r="H37" s="11"/>
-      <c r="I37" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="J37" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K37" s="7"/>
+      <c r="I37" s="11"/>
+      <c r="J37" s="11"/>
+      <c r="K37" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="L37" s="7"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E38" s="9"/>
-      <c r="F38" s="8" t="n">
+      <c r="F38" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G38" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="G38" s="10" t="n">
+      <c r="H38" s="10" t="n">
         <v>0.6</v>
       </c>
-      <c r="H38" s="11"/>
-      <c r="I38" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="J38" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K38" s="7"/>
+      <c r="I38" s="11"/>
+      <c r="J38" s="11"/>
+      <c r="K38" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="L38" s="7"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B39" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H39" s="2" t="n">
+        <v>60.8</v>
+      </c>
+      <c r="K39" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G39" s="2" t="n">
-        <v>60.8</v>
-      </c>
-      <c r="J39" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E40" s="9"/>
-      <c r="F40" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="G40" s="10" t="n">
+      <c r="F40" s="7"/>
+      <c r="G40" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H40" s="10" t="n">
         <v>130</v>
       </c>
-      <c r="H40" s="11"/>
-      <c r="I40" s="7"/>
-      <c r="J40" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K40" s="7"/>
+      <c r="I40" s="11"/>
+      <c r="J40" s="11"/>
+      <c r="K40" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="L40" s="7"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E41" s="9"/>
-      <c r="F41" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="G41" s="10" t="n">
+      <c r="F41" s="7"/>
+      <c r="G41" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H41" s="10" t="n">
         <v>1777</v>
       </c>
-      <c r="H41" s="11"/>
-      <c r="I41" s="7"/>
-      <c r="J41" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K41" s="7"/>
+      <c r="I41" s="11"/>
+      <c r="J41" s="11"/>
+      <c r="K41" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="L41" s="7"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C42" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D42" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="D42" s="9" t="s">
-        <v>47</v>
-      </c>
       <c r="E42" s="9"/>
-      <c r="F42" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="G42" s="10" t="n">
+      <c r="F42" s="7"/>
+      <c r="G42" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H42" s="10" t="n">
         <v>4000</v>
       </c>
-      <c r="H42" s="11"/>
-      <c r="I42" s="7"/>
-      <c r="J42" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K42" s="7"/>
+      <c r="I42" s="11"/>
+      <c r="J42" s="11"/>
+      <c r="K42" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="L42" s="7"/>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E43" s="9"/>
-      <c r="F43" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="G43" s="10" t="n">
+      <c r="F43" s="7"/>
+      <c r="G43" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H43" s="10" t="n">
         <v>100</v>
       </c>
-      <c r="H43" s="11"/>
-      <c r="I43" s="7"/>
-      <c r="J43" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K43" s="7"/>
+      <c r="I43" s="11"/>
+      <c r="J43" s="11"/>
+      <c r="K43" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="L43" s="7"/>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E44" s="9"/>
-      <c r="F44" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="G44" s="10" t="n">
+      <c r="F44" s="7"/>
+      <c r="G44" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H44" s="10" t="n">
         <v>180</v>
       </c>
-      <c r="H44" s="11"/>
-      <c r="I44" s="7"/>
-      <c r="J44" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K44" s="7"/>
+      <c r="I44" s="11"/>
+      <c r="J44" s="11"/>
+      <c r="K44" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="L44" s="7"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G45" s="2" t="n">
+        <v>51</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H45" s="2" t="n">
         <v>38</v>
       </c>
-      <c r="J45" s="1" t="s">
-        <v>15</v>
+      <c r="K45" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F46" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="G46" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="G46" s="2" t="n">
+      <c r="H46" s="2" t="n">
         <v>0.03</v>
       </c>
-      <c r="J46" s="1" t="s">
-        <v>15</v>
+      <c r="K46" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B47" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G47" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H47" s="2" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="K47" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F47" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="G47" s="2" t="n">
-        <v>0.03</v>
-      </c>
-      <c r="J47" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E48" s="9"/>
-      <c r="F48" s="8" t="n">
+      <c r="F48" s="7"/>
+      <c r="G48" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="G48" s="10" t="n">
+      <c r="H48" s="10" t="n">
         <v>0.03</v>
       </c>
-      <c r="H48" s="11"/>
-      <c r="I48" s="7"/>
-      <c r="J48" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K48" s="7"/>
+      <c r="I48" s="11"/>
+      <c r="J48" s="11"/>
+      <c r="K48" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="L48" s="7"/>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E49" s="9"/>
-      <c r="F49" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="G49" s="10" t="n">
+      <c r="F49" s="7"/>
+      <c r="G49" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H49" s="10" t="n">
         <v>35</v>
       </c>
-      <c r="H49" s="11"/>
-      <c r="I49" s="7"/>
-      <c r="J49" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K49" s="7"/>
+      <c r="I49" s="11"/>
+      <c r="J49" s="11"/>
+      <c r="K49" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="L49" s="7"/>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D50" s="9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E50" s="9"/>
-      <c r="F50" s="8" t="n">
+      <c r="F50" s="7"/>
+      <c r="G50" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="G50" s="10" t="n">
+      <c r="H50" s="10" t="n">
         <v>0.03</v>
       </c>
-      <c r="H50" s="11"/>
-      <c r="I50" s="7"/>
-      <c r="J50" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K50" s="7"/>
+      <c r="I50" s="11"/>
+      <c r="J50" s="11"/>
+      <c r="K50" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="L50" s="7"/>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D51" s="9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E51" s="9"/>
-      <c r="F51" s="8" t="n">
+      <c r="F51" s="7"/>
+      <c r="G51" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="G51" s="10" t="n">
+      <c r="H51" s="10" t="n">
         <v>0.03</v>
       </c>
-      <c r="H51" s="11"/>
-      <c r="I51" s="7"/>
-      <c r="J51" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K51" s="7"/>
+      <c r="I51" s="11"/>
+      <c r="J51" s="11"/>
+      <c r="K51" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="L51" s="7"/>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D52" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E52" s="9"/>
-      <c r="F52" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G52" s="10" t="n">
+      <c r="F52" s="7"/>
+      <c r="G52" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H52" s="10" t="n">
         <v>20</v>
       </c>
-      <c r="H52" s="11"/>
-      <c r="I52" s="7"/>
-      <c r="J52" s="7" t="s">
-        <v>53</v>
-      </c>
+      <c r="I52" s="11"/>
+      <c r="J52" s="11"/>
       <c r="K52" s="7" t="s">
         <v>54</v>
       </c>
+      <c r="L52" s="7" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D53" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E53" s="9"/>
+      <c r="F53" s="7"/>
+      <c r="G53" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H53" s="10" t="n">
         <v>30</v>
       </c>
-      <c r="E53" s="9"/>
-      <c r="F53" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G53" s="10" t="n">
-        <v>30</v>
-      </c>
-      <c r="H53" s="11" t="n">
+      <c r="I53" s="11"/>
+      <c r="J53" s="11" t="n">
         <v>2025</v>
       </c>
-      <c r="I53" s="7"/>
-      <c r="J53" s="7" t="s">
+      <c r="K53" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="L53" s="7" t="s">
         <v>55</v>
-      </c>
-      <c r="K53" s="7" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D54" s="9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E54" s="9"/>
-      <c r="F54" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G54" s="10" t="n">
+      <c r="F54" s="7"/>
+      <c r="G54" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H54" s="10" t="n">
         <v>20</v>
       </c>
-      <c r="H54" s="12" t="n">
+      <c r="I54" s="12"/>
+      <c r="J54" s="12" t="n">
         <v>2050</v>
       </c>
-      <c r="I54" s="7"/>
-      <c r="J54" s="7" t="s">
+      <c r="K54" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="L54" s="7" t="s">
         <v>55</v>
-      </c>
-      <c r="K54" s="7" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D55" s="9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E55" s="9"/>
-      <c r="F55" s="1" t="s">
+      <c r="F55" s="7"/>
+      <c r="G55" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H55" s="10" t="n">
         <v>14</v>
       </c>
-      <c r="G55" s="10" t="n">
-        <v>14</v>
-      </c>
-      <c r="H55" s="11"/>
-      <c r="I55" s="7"/>
-      <c r="J55" s="7" t="s">
-        <v>53</v>
-      </c>
+      <c r="I55" s="11"/>
+      <c r="J55" s="11"/>
       <c r="K55" s="7" t="s">
         <v>54</v>
       </c>
+      <c r="L55" s="7" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D56" s="9" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E56" s="9"/>
-      <c r="F56" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G56" s="10" t="n">
+      <c r="F56" s="7"/>
+      <c r="G56" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H56" s="10" t="n">
         <v>30</v>
       </c>
-      <c r="H56" s="11"/>
-      <c r="I56" s="7"/>
-      <c r="J56" s="7" t="s">
-        <v>53</v>
-      </c>
+      <c r="I56" s="11"/>
+      <c r="J56" s="11"/>
       <c r="K56" s="7" t="s">
         <v>54</v>
       </c>
+      <c r="L56" s="7" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="6"/>
@@ -5024,13 +5080,12 @@
     <row r="1037" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1037" s="6"/>
     </row>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <autoFilter ref="A1:K37"/>
+  <autoFilter ref="A:L"/>
   <dataValidations count="1">
     <dataValidation allowBlank="true" error="Check value!" errorTitle="Check value!" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="A1:A1037" type="list">
-      <formula1>#REF!</formula1>
+      <formula1>#ref!</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -5059,7 +5114,7 @@
       <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.23"/>
@@ -5067,30 +5122,30 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="13" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>60</v>
@@ -5101,13 +5156,13 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>62</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>61</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>30</v>
@@ -5118,13 +5173,13 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>40</v>
@@ -5135,13 +5190,13 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>100</v>
@@ -5152,13 +5207,13 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>60</v>
@@ -5169,13 +5224,13 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>100</v>
@@ -5186,13 +5241,13 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>50</v>
@@ -5203,13 +5258,13 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="0" t="s">
         <v>62</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>61</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>15</v>
@@ -5220,13 +5275,13 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>30</v>
@@ -5237,13 +5292,13 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>60</v>
@@ -5254,13 +5309,13 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>40</v>
@@ -5271,13 +5326,13 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>300</v>
@@ -5302,78 +5357,99 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topLeft" activeCell="H28" activeCellId="0" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.21"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="13" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B6" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" s="0" t="s">
         <v>77</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -5394,11 +5470,11 @@
   </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="13.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.69"/>
@@ -5409,69 +5485,69 @@
         <v>0</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated framework for urea data.
</commit_message>
<xml_diff>
--- a/input/data/data.xlsx
+++ b/input/data/data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="technology_data" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,8 +14,8 @@
     <sheet name="routes" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">technology_data!$A$1:$L$66</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">technology_data!$A$1:$L$38</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">technology_data!$A$1:$L$69</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">technology_data!$A$1:$L$41</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="122">
   <si>
     <t xml:space="preserve">process_group</t>
   </si>
@@ -89,30 +89,45 @@
     <t xml:space="preserve">hydrogen</t>
   </si>
   <si>
+    <t xml:space="preserve">MWh/t</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boulamanti and Moya (2017)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHECK VALUE!!! @Lukas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">electricity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">natural gas</t>
+  </si>
+  <si>
     <t xml:space="preserve">t/t</t>
   </si>
   <si>
-    <t xml:space="preserve">Boulamanti and Moya (2017)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">electricity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">natural gas</t>
-  </si>
-  <si>
     <t xml:space="preserve">fixed_opex</t>
   </si>
   <si>
     <t xml:space="preserve">without hydrogen</t>
   </si>
   <si>
+    <t xml:space="preserve">DAC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test value</t>
+  </si>
+  <si>
     <t xml:space="preserve">UREA</t>
   </si>
   <si>
     <t xml:space="preserve">feedstock_demand</t>
   </si>
   <si>
+    <t xml:space="preserve">co2</t>
+  </si>
+  <si>
     <t xml:space="preserve">ammonia</t>
   </si>
   <si>
@@ -161,9 +176,6 @@
     <t xml:space="preserve">coke</t>
   </si>
   <si>
-    <t xml:space="preserve">MWh/t</t>
-  </si>
-  <si>
     <t xml:space="preserve">H2</t>
   </si>
   <si>
@@ -318,6 +330,9 @@
   </si>
   <si>
     <t xml:space="preserve">Integrated ammonia plant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Direct-air capture</t>
   </si>
   <si>
     <t xml:space="preserve">processes</t>
@@ -383,13 +398,19 @@
     <t xml:space="preserve">1: none</t>
   </si>
   <si>
-    <t xml:space="preserve">ELEC_HB_UREA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ELEC, HB, UREA</t>
+    <t xml:space="preserve">ELEC_HB_DAC_UREA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ELEC, HB, DAC, UREA</t>
   </si>
   <si>
     <t xml:space="preserve">1: none, 2: hydrogen, 3: ammonia, 4: urea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ELEC_HB_CCU_UREA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ELEC, HB, CCU, UREA</t>
   </si>
 </sst>
 </file>
@@ -647,10 +668,10 @@
     <tabColor rgb="FFDEEBF7"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L1030"/>
+  <dimension ref="A1:L1033"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B69" activeCellId="0" sqref="B69"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -764,10 +785,13 @@
         <v>20</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>0.178</v>
+        <v>5.9</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>21</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -781,7 +805,10 @@
         <v>18</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -795,10 +822,10 @@
         <v>18</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="H6" s="2" t="n">
         <v>0.65</v>
@@ -815,7 +842,7 @@
         <v>13</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>15</v>
@@ -827,7 +854,7 @@
         <v>16</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -838,7 +865,7 @@
         <v>17</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>15</v>
@@ -855,19 +882,23 @@
         <v>12</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>20</v>
       </c>
       <c r="H9" s="2" t="n">
-        <v>0.6</v>
+        <v>2</v>
+      </c>
+      <c r="I9" s="0"/>
+      <c r="L9" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -875,19 +906,20 @@
         <v>12</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="H10" s="2" t="n">
-        <v>0.5</v>
+        <v>300</v>
+      </c>
+      <c r="I10" s="0"/>
+      <c r="L10" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -895,445 +927,429 @@
         <v>12</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C11" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H11" s="2" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H12" s="2" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" s="2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H11" s="2" t="n">
+      <c r="H14" s="2" t="n">
         <v>300</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="8" t="s">
+      <c r="L14" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="H12" s="10" t="n">
-        <v>800000</v>
-      </c>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11" t="n">
-        <v>2025</v>
-      </c>
-      <c r="K12" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="L12" s="8"/>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="H13" s="10" t="n">
-        <v>300000</v>
-      </c>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12" t="n">
-        <v>2050</v>
-      </c>
-      <c r="K13" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="L13" s="8"/>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E14" s="9"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H14" s="10" t="n">
-        <v>1.47</v>
-      </c>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12" t="n">
-        <v>2025</v>
-      </c>
-      <c r="K14" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="L14" s="8"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="8" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>22</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D15" s="9"/>
       <c r="E15" s="9"/>
       <c r="F15" s="8"/>
-      <c r="G15" s="7" t="n">
-        <v>1</v>
+      <c r="G15" s="7" t="s">
+        <v>36</v>
       </c>
       <c r="H15" s="10" t="n">
-        <v>1.33</v>
-      </c>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12" t="n">
-        <v>2050</v>
-      </c>
-      <c r="K15" s="8"/>
+        <v>800000</v>
+      </c>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11" t="n">
+        <v>2025</v>
+      </c>
+      <c r="K15" s="8" t="s">
+        <v>37</v>
+      </c>
       <c r="L15" s="8"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="8" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>33</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D16" s="9"/>
       <c r="E16" s="9"/>
       <c r="F16" s="8"/>
-      <c r="G16" s="7" t="n">
+      <c r="G16" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H16" s="10" t="n">
+        <v>300000</v>
+      </c>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12" t="n">
+        <v>2050</v>
+      </c>
+      <c r="K16" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L16" s="8"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" s="9"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="H16" s="10" t="n">
-        <v>0.03</v>
-      </c>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="8" t="s">
+      <c r="H17" s="10" t="n">
+        <v>1.47</v>
+      </c>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12" t="n">
+        <v>2025</v>
+      </c>
+      <c r="K17" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L17" s="8"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="L16" s="8"/>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="6" t="s">
+      <c r="B18" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H17" s="2" t="n">
-        <v>106</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H18" s="2" t="n">
-        <v>64</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="C18" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" s="9"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="H18" s="10" t="n">
+        <v>1.33</v>
+      </c>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12" t="n">
+        <v>2050</v>
+      </c>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="C19" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D19" s="9"/>
       <c r="E19" s="9"/>
       <c r="F19" s="8"/>
-      <c r="G19" s="7" t="s">
-        <v>15</v>
+      <c r="G19" s="7" t="n">
+        <v>1</v>
       </c>
       <c r="H19" s="10" t="n">
-        <v>230</v>
+        <v>0.03</v>
       </c>
       <c r="I19" s="11"/>
-      <c r="J19" s="11" t="n">
-        <v>2025</v>
-      </c>
+      <c r="J19" s="11"/>
       <c r="K19" s="8" t="s">
         <v>39</v>
       </c>
       <c r="L19" s="8"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C20" s="7" t="s">
+      <c r="A20" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="7" t="s">
+      <c r="G20" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H20" s="10" t="n">
+      <c r="H20" s="2" t="n">
+        <v>106</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H21" s="2" t="n">
+        <v>64</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H22" s="10" t="n">
+        <v>230</v>
+      </c>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11" t="n">
+        <v>2025</v>
+      </c>
+      <c r="K22" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="L22" s="8"/>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H23" s="10" t="n">
         <v>200</v>
       </c>
-      <c r="I20" s="12"/>
-      <c r="J20" s="12" t="n">
+      <c r="I23" s="12"/>
+      <c r="J23" s="12" t="n">
         <v>2050</v>
       </c>
-      <c r="K20" s="8" t="s">
+      <c r="K23" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="L23" s="8"/>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="L20" s="8"/>
-    </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B21" s="8" t="s">
+      <c r="B24" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H24" s="10" t="n">
+        <v>184</v>
+      </c>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="L24" s="8"/>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="H21" s="10" t="n">
-        <v>184</v>
-      </c>
-      <c r="I21" s="11"/>
-      <c r="J21" s="11"/>
-      <c r="K21" s="8" t="s">
+      <c r="C25" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G25" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H25" s="2" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="K25" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="L21" s="8"/>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C22" s="1" t="s">
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G22" s="1" t="n">
+      <c r="D26" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G26" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="H22" s="2" t="n">
+      <c r="H26" s="2" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H27" s="2" t="n">
         <v>0.17</v>
       </c>
-      <c r="K22" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G23" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="H23" s="2" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="K23" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H24" s="2" t="n">
-        <v>0.17</v>
-      </c>
-      <c r="K24" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E25" s="9"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="H25" s="10" t="n">
-        <v>0.329</v>
-      </c>
-      <c r="I25" s="11"/>
-      <c r="J25" s="11"/>
-      <c r="K25" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="L25" s="8"/>
-    </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B26" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E26" s="9"/>
-      <c r="F26" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="G26" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="H26" s="10" t="n">
-        <v>1.69983</v>
-      </c>
-      <c r="I26" s="11"/>
-      <c r="J26" s="11"/>
-      <c r="K26" s="8" t="s">
+      <c r="K27" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="L26" s="8"/>
-    </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E27" s="9"/>
-      <c r="F27" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="G27" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="H27" s="10" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="I27" s="11"/>
-      <c r="J27" s="11"/>
-      <c r="K27" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="L27" s="8"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="8" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C28" s="7" t="s">
         <v>18</v>
@@ -1342,504 +1358,504 @@
         <v>23</v>
       </c>
       <c r="E28" s="9"/>
-      <c r="F28" s="6" t="s">
-        <v>46</v>
-      </c>
+      <c r="F28" s="8"/>
       <c r="G28" s="7" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="H28" s="10" t="n">
-        <v>2.79</v>
+        <v>0.329</v>
       </c>
       <c r="I28" s="11"/>
       <c r="J28" s="11"/>
       <c r="K28" s="8" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="L28" s="8"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="8" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C29" s="7" t="s">
         <v>18</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E29" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="F29" s="8" t="s">
-        <v>48</v>
+        <v>19</v>
+      </c>
+      <c r="E29" s="9"/>
+      <c r="F29" s="6" t="s">
+        <v>49</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="H29" s="10" t="n">
-        <v>0.753</v>
+        <v>1.69983</v>
       </c>
       <c r="I29" s="11"/>
       <c r="J29" s="11"/>
       <c r="K29" s="8" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="L29" s="8"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="8" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>18</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E30" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E30" s="9"/>
+      <c r="F30" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="F30" s="8" t="s">
-        <v>50</v>
-      </c>
       <c r="G30" s="7" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="H30" s="10" t="n">
-        <v>0.667</v>
+        <v>0.5</v>
       </c>
       <c r="I30" s="11"/>
       <c r="J30" s="11"/>
       <c r="K30" s="8" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="L30" s="8"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="8" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C31" s="7" t="s">
         <v>18</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E31" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="F31" s="8"/>
+        <v>24</v>
+      </c>
+      <c r="E31" s="9"/>
+      <c r="F31" s="6" t="s">
+        <v>50</v>
+      </c>
       <c r="G31" s="7" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="H31" s="10" t="n">
-        <v>0.159</v>
+        <v>2.79</v>
       </c>
       <c r="I31" s="11"/>
       <c r="J31" s="11"/>
       <c r="K31" s="8" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="L31" s="8"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C32" s="1" t="s">
+      <c r="A32" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="F32" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="D32" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H32" s="2" t="n">
-        <v>110</v>
-      </c>
-      <c r="K32" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="G32" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H32" s="10" t="n">
+        <v>0.753</v>
+      </c>
+      <c r="I32" s="11"/>
+      <c r="J32" s="11"/>
+      <c r="K32" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="L32" s="8"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H33" s="2" t="n">
-        <v>143</v>
-      </c>
-      <c r="K33" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="A33" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H33" s="10" t="n">
+        <v>0.667</v>
+      </c>
+      <c r="I33" s="11"/>
+      <c r="J33" s="11"/>
+      <c r="K33" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="L33" s="8"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G34" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="H34" s="2" t="n">
-        <v>0.278</v>
-      </c>
-      <c r="K34" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="A34" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="F34" s="8"/>
+      <c r="G34" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H34" s="10" t="n">
+        <v>0.159</v>
+      </c>
+      <c r="I34" s="11"/>
+      <c r="J34" s="11"/>
+      <c r="K34" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="L34" s="8"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="6" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>27</v>
+        <v>56</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G35" s="1" t="n">
-        <v>1</v>
+        <v>47</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="H35" s="2" t="n">
-        <v>1.5</v>
+        <v>110</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B36" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C36" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D36" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="E36" s="9"/>
-      <c r="F36" s="8"/>
-      <c r="G36" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H36" s="10" t="n">
-        <v>0.011</v>
-      </c>
-      <c r="I36" s="11"/>
-      <c r="J36" s="11"/>
-      <c r="K36" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="L36" s="8"/>
+      <c r="A36" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H36" s="2" t="n">
+        <v>143</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="6" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G37" s="1" t="n">
         <v>1</v>
       </c>
       <c r="H37" s="2" t="n">
-        <v>0.18</v>
+        <v>0.278</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B38" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C38" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D38" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="E38" s="9"/>
-      <c r="F38" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="G38" s="7" t="n">
+      <c r="A38" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G38" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="H38" s="10" t="n">
-        <v>0.85</v>
-      </c>
-      <c r="I38" s="11"/>
-      <c r="J38" s="11"/>
-      <c r="K38" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="L38" s="8"/>
+      <c r="H38" s="2" t="n">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="8" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E39" s="9"/>
-      <c r="F39" s="8" t="s">
-        <v>50</v>
-      </c>
+      <c r="F39" s="8"/>
       <c r="G39" s="7" t="n">
         <v>1</v>
       </c>
       <c r="H39" s="10" t="n">
-        <v>0.35</v>
+        <v>0.011</v>
       </c>
       <c r="I39" s="11"/>
       <c r="J39" s="11"/>
       <c r="K39" s="8" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="L39" s="8"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B40" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C40" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D40" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="E40" s="9"/>
-      <c r="F40" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="G40" s="7" t="n">
+      <c r="A40" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G40" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="H40" s="10" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="I40" s="11"/>
-      <c r="J40" s="11"/>
-      <c r="K40" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="L40" s="8"/>
+      <c r="H40" s="2" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="8" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="E41" s="9"/>
       <c r="F41" s="8" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G41" s="7" t="n">
         <v>1</v>
       </c>
       <c r="H41" s="10" t="n">
-        <v>0.6</v>
+        <v>0.85</v>
       </c>
       <c r="I41" s="11"/>
       <c r="J41" s="11"/>
       <c r="K41" s="8" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="L41" s="8"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="8" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D42" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="E42" s="9"/>
+      <c r="F42" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="E42" s="9"/>
-      <c r="F42" s="8"/>
       <c r="G42" s="7" t="n">
         <v>1</v>
       </c>
       <c r="H42" s="10" t="n">
-        <v>1.504</v>
+        <v>0.35</v>
       </c>
       <c r="I42" s="11"/>
       <c r="J42" s="11"/>
       <c r="K42" s="8" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="L42" s="8"/>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="8" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="E43" s="9"/>
-      <c r="F43" s="8"/>
+      <c r="F43" s="8" t="s">
+        <v>52</v>
+      </c>
       <c r="G43" s="7" t="n">
         <v>1</v>
       </c>
       <c r="H43" s="10" t="n">
-        <v>0.011</v>
+        <v>0.1</v>
       </c>
       <c r="I43" s="11"/>
       <c r="J43" s="11"/>
       <c r="K43" s="8" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="L43" s="8"/>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="8" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E44" s="9"/>
       <c r="F44" s="8" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="G44" s="7" t="n">
         <v>1</v>
       </c>
       <c r="H44" s="10" t="n">
-        <v>0.85</v>
+        <v>0.6</v>
       </c>
       <c r="I44" s="11"/>
       <c r="J44" s="11"/>
       <c r="K44" s="8" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="L44" s="8"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="8" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E45" s="9"/>
-      <c r="F45" s="8" t="s">
-        <v>50</v>
-      </c>
+      <c r="F45" s="8"/>
       <c r="G45" s="7" t="n">
         <v>1</v>
       </c>
       <c r="H45" s="10" t="n">
-        <v>0.35</v>
+        <v>1.504</v>
       </c>
       <c r="I45" s="11"/>
       <c r="J45" s="11"/>
       <c r="K45" s="8" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="L45" s="8"/>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="8" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E46" s="9"/>
       <c r="F46" s="8"/>
@@ -1847,222 +1863,226 @@
         <v>1</v>
       </c>
       <c r="H46" s="10" t="n">
-        <v>0.002</v>
+        <v>0.011</v>
       </c>
       <c r="I46" s="11"/>
       <c r="J46" s="11"/>
       <c r="K46" s="8" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="L46" s="8"/>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="8" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D47" s="9" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="E47" s="9"/>
-      <c r="F47" s="8"/>
+      <c r="F47" s="8" t="s">
+        <v>52</v>
+      </c>
       <c r="G47" s="7" t="n">
         <v>1</v>
       </c>
       <c r="H47" s="10" t="n">
-        <v>0.05</v>
+        <v>0.85</v>
       </c>
       <c r="I47" s="11"/>
       <c r="J47" s="11"/>
       <c r="K47" s="8" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="L47" s="8"/>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="8" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="E48" s="9"/>
       <c r="F48" s="8" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="G48" s="7" t="n">
         <v>1</v>
       </c>
       <c r="H48" s="10" t="n">
-        <v>0.1</v>
+        <v>0.35</v>
       </c>
       <c r="I48" s="11"/>
       <c r="J48" s="11"/>
       <c r="K48" s="8" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="L48" s="8"/>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="8" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="E49" s="9"/>
-      <c r="F49" s="8" t="s">
-        <v>50</v>
-      </c>
+      <c r="F49" s="8"/>
       <c r="G49" s="7" t="n">
         <v>1</v>
       </c>
       <c r="H49" s="10" t="n">
-        <v>0.6</v>
+        <v>0.002</v>
       </c>
       <c r="I49" s="11"/>
       <c r="J49" s="11"/>
       <c r="K49" s="8" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="L49" s="8"/>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="G50" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H50" s="2" t="n">
-        <v>60.8</v>
-      </c>
-      <c r="K50" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="A50" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D50" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E50" s="9"/>
+      <c r="F50" s="8"/>
+      <c r="G50" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="H50" s="10" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="I50" s="11"/>
+      <c r="J50" s="11"/>
+      <c r="K50" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="L50" s="8"/>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="8" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>61</v>
+        <v>31</v>
       </c>
       <c r="D51" s="9" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="E51" s="9"/>
-      <c r="F51" s="8"/>
-      <c r="G51" s="7" t="s">
-        <v>15</v>
+      <c r="F51" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="G51" s="7" t="n">
+        <v>1</v>
       </c>
       <c r="H51" s="10" t="n">
-        <v>130</v>
+        <v>0.1</v>
       </c>
       <c r="I51" s="11"/>
       <c r="J51" s="11"/>
       <c r="K51" s="8" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="L51" s="8"/>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="8" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>61</v>
+        <v>31</v>
       </c>
       <c r="D52" s="9" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="E52" s="9"/>
-      <c r="F52" s="8"/>
-      <c r="G52" s="7" t="s">
-        <v>15</v>
+      <c r="F52" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="G52" s="7" t="n">
+        <v>1</v>
       </c>
       <c r="H52" s="10" t="n">
-        <v>1777</v>
+        <v>0.6</v>
       </c>
       <c r="I52" s="11"/>
       <c r="J52" s="11"/>
       <c r="K52" s="8" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="L52" s="8"/>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B53" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C53" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="D53" s="9" t="s">
+      <c r="A53" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D53" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E53" s="9"/>
-      <c r="F53" s="8"/>
-      <c r="G53" s="7" t="s">
+      <c r="G53" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H53" s="10" t="n">
-        <v>4000</v>
-      </c>
-      <c r="I53" s="11"/>
-      <c r="J53" s="11"/>
-      <c r="K53" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="L53" s="8"/>
+      <c r="H53" s="2" t="n">
+        <v>60.8</v>
+      </c>
+      <c r="K53" s="1" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="8" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="D54" s="9" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="E54" s="9"/>
       <c r="F54" s="8"/>
@@ -2070,27 +2090,27 @@
         <v>15</v>
       </c>
       <c r="H54" s="10" t="n">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="I54" s="11"/>
       <c r="J54" s="11"/>
       <c r="K54" s="8" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="L54" s="8"/>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="8" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="D55" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E55" s="9"/>
       <c r="F55" s="8"/>
@@ -2098,274 +2118,264 @@
         <v>15</v>
       </c>
       <c r="H55" s="10" t="n">
-        <v>180</v>
+        <v>1777</v>
       </c>
       <c r="I55" s="11"/>
       <c r="J55" s="11"/>
       <c r="K55" s="8" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="L55" s="8"/>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D56" s="1" t="s">
+      <c r="A56" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B56" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C56" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D56" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="E56" s="9"/>
+      <c r="F56" s="8"/>
+      <c r="G56" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H56" s="10" t="n">
+        <v>4000</v>
+      </c>
+      <c r="I56" s="11"/>
+      <c r="J56" s="11"/>
+      <c r="K56" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="L56" s="8"/>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B57" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C57" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D57" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E57" s="9"/>
+      <c r="F57" s="8"/>
+      <c r="G57" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H57" s="10" t="n">
+        <v>100</v>
+      </c>
+      <c r="I57" s="11"/>
+      <c r="J57" s="11"/>
+      <c r="K57" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="L57" s="8"/>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C58" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D58" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="G56" s="1" t="s">
+      <c r="E58" s="9"/>
+      <c r="F58" s="8"/>
+      <c r="G58" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="H56" s="2" t="n">
+      <c r="H58" s="10" t="n">
+        <v>180</v>
+      </c>
+      <c r="I58" s="11"/>
+      <c r="J58" s="11"/>
+      <c r="K58" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="L58" s="8"/>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H59" s="2" t="n">
         <v>38</v>
       </c>
-      <c r="K56" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G57" s="1" t="n">
+      <c r="K59" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G60" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="H57" s="2" t="n">
+      <c r="H60" s="2" t="n">
         <v>0.03</v>
       </c>
-      <c r="K57" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G58" s="1" t="n">
+      <c r="K60" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G61" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="H58" s="2" t="n">
+      <c r="H61" s="2" t="n">
         <v>0.03</v>
       </c>
-      <c r="K58" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B59" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C59" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D59" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E59" s="9"/>
-      <c r="F59" s="8"/>
-      <c r="G59" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H59" s="10" t="n">
-        <v>0.03</v>
-      </c>
-      <c r="I59" s="11"/>
-      <c r="J59" s="11"/>
-      <c r="K59" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="L59" s="8"/>
-    </row>
-    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B60" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C60" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D60" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="E60" s="9"/>
-      <c r="F60" s="8"/>
-      <c r="G60" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="H60" s="10" t="n">
-        <v>35</v>
-      </c>
-      <c r="I60" s="11"/>
-      <c r="J60" s="11"/>
-      <c r="K60" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="L60" s="8"/>
-    </row>
-    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B61" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C61" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D61" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E61" s="9"/>
-      <c r="F61" s="8"/>
-      <c r="G61" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H61" s="10" t="n">
-        <v>0.03</v>
-      </c>
-      <c r="I61" s="11"/>
-      <c r="J61" s="11"/>
-      <c r="K61" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="L61" s="8"/>
+      <c r="K61" s="1" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="8" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B62" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C62" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D62" s="9" t="s">
         <v>38</v>
-      </c>
-      <c r="C62" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D62" s="9" t="s">
-        <v>59</v>
       </c>
       <c r="E62" s="9"/>
       <c r="F62" s="8"/>
-      <c r="G62" s="1" t="s">
-        <v>15</v>
+      <c r="G62" s="7" t="n">
+        <v>1</v>
       </c>
       <c r="H62" s="10" t="n">
-        <v>20</v>
+        <v>0.03</v>
       </c>
       <c r="I62" s="11"/>
       <c r="J62" s="11"/>
       <c r="K62" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="L62" s="8" t="s">
-        <v>65</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="L62" s="8"/>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="8" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>63</v>
+        <v>26</v>
       </c>
       <c r="D63" s="9" t="s">
-        <v>19</v>
+        <v>66</v>
       </c>
       <c r="E63" s="9"/>
       <c r="F63" s="8"/>
-      <c r="G63" s="1" t="s">
+      <c r="G63" s="7" t="s">
         <v>15</v>
       </c>
       <c r="H63" s="10" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="I63" s="11"/>
-      <c r="J63" s="11" t="n">
-        <v>2025</v>
-      </c>
+      <c r="J63" s="11"/>
       <c r="K63" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="L63" s="8" t="s">
-        <v>65</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="L63" s="8"/>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="8" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="B64" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C64" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D64" s="9" t="s">
         <v>38</v>
-      </c>
-      <c r="C64" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D64" s="9" t="s">
-        <v>19</v>
       </c>
       <c r="E64" s="9"/>
       <c r="F64" s="8"/>
-      <c r="G64" s="1" t="s">
-        <v>15</v>
+      <c r="G64" s="7" t="n">
+        <v>1</v>
       </c>
       <c r="H64" s="10" t="n">
-        <v>20</v>
-      </c>
-      <c r="I64" s="12"/>
-      <c r="J64" s="12" t="n">
-        <v>2050</v>
-      </c>
+        <v>0.03</v>
+      </c>
+      <c r="I64" s="11"/>
+      <c r="J64" s="11"/>
       <c r="K64" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="L64" s="8" t="s">
-        <v>65</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="L64" s="8"/>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="8" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C65" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D65" s="9" t="s">
         <v>63</v>
-      </c>
-      <c r="D65" s="9" t="s">
-        <v>54</v>
       </c>
       <c r="E65" s="9"/>
       <c r="F65" s="8"/>
@@ -2373,29 +2383,29 @@
         <v>15</v>
       </c>
       <c r="H65" s="10" t="n">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="I65" s="11"/>
       <c r="J65" s="11"/>
       <c r="K65" s="8" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="L65" s="8" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D66" s="9" t="s">
-        <v>67</v>
+        <v>19</v>
       </c>
       <c r="E66" s="9"/>
       <c r="F66" s="8"/>
@@ -2406,26 +2416,28 @@
         <v>30</v>
       </c>
       <c r="I66" s="11"/>
-      <c r="J66" s="11"/>
+      <c r="J66" s="11" t="n">
+        <v>2025</v>
+      </c>
       <c r="K66" s="8" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="L66" s="8" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="8" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D67" s="9" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="E67" s="9"/>
       <c r="F67" s="8"/>
@@ -2435,19 +2447,29 @@
       <c r="H67" s="10" t="n">
         <v>20</v>
       </c>
+      <c r="I67" s="12"/>
+      <c r="J67" s="12" t="n">
+        <v>2050</v>
+      </c>
+      <c r="K67" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="L67" s="8" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="8" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="B68" s="8" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D68" s="9" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="E68" s="9"/>
       <c r="F68" s="8"/>
@@ -2455,21 +2477,29 @@
         <v>15</v>
       </c>
       <c r="H68" s="10" t="n">
-        <v>20</v>
+        <v>14</v>
+      </c>
+      <c r="I68" s="11"/>
+      <c r="J68" s="11"/>
+      <c r="K68" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="L68" s="8" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="8" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D69" s="9" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E69" s="9"/>
       <c r="F69" s="8"/>
@@ -2477,17 +2507,91 @@
         <v>15</v>
       </c>
       <c r="H69" s="10" t="n">
+        <v>30</v>
+      </c>
+      <c r="I69" s="11"/>
+      <c r="J69" s="11"/>
+      <c r="K69" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="L69" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B70" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C70" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D70" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E70" s="9"/>
+      <c r="F70" s="8"/>
+      <c r="G70" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H70" s="10" t="n">
         <v>20</v>
       </c>
-    </row>
-    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="6"/>
+      <c r="L70" s="3" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="6"/>
+      <c r="A71" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B71" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C71" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D71" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E71" s="9"/>
+      <c r="F71" s="8"/>
+      <c r="G71" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H71" s="10" t="n">
+        <v>20</v>
+      </c>
+      <c r="L71" s="3" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="6"/>
+      <c r="A72" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B72" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C72" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D72" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="E72" s="9"/>
+      <c r="F72" s="8"/>
+      <c r="G72" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H72" s="10" t="n">
+        <v>20</v>
+      </c>
+      <c r="L72" s="3" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="6"/>
@@ -5363,10 +5467,19 @@
     <row r="1030" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1030" s="6"/>
     </row>
+    <row r="1031" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1031" s="6"/>
+    </row>
+    <row r="1032" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1032" s="6"/>
+    </row>
+    <row r="1033" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1033" s="6"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:L66"/>
+  <autoFilter ref="A1:L69"/>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" error="Check value!" errorTitle="Check value!" operator="between" showDropDown="true" showErrorMessage="true" showInputMessage="true" sqref="A1:A1069" type="none">
+    <dataValidation allowBlank="true" error="Check value!" errorTitle="Check value!" operator="between" showDropDown="true" showErrorMessage="true" showInputMessage="true" sqref="A1:A1072" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -5390,7 +5503,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
+      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5401,10 +5514,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="13" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C1" s="13" t="s">
         <v>6</v>
@@ -5418,13 +5531,13 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>60</v>
@@ -5435,13 +5548,13 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>30</v>
@@ -5452,13 +5565,13 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="B4" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>77</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>73</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>40</v>
@@ -5469,13 +5582,13 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>100</v>
@@ -5486,13 +5599,13 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>60</v>
@@ -5503,10 +5616,10 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>15</v>
@@ -5520,13 +5633,13 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>50</v>
@@ -5537,13 +5650,13 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>15</v>
@@ -5554,13 +5667,13 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="B10" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="C10" s="0" t="s">
         <v>77</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>73</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>30</v>
@@ -5571,13 +5684,13 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>60</v>
@@ -5588,13 +5701,13 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>40</v>
@@ -5605,10 +5718,10 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>15</v>
@@ -5620,6 +5733,7 @@
         <v>2050</v>
       </c>
     </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -5637,10 +5751,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5650,13 +5764,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="13" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="D1" s="13" t="s">
         <v>6</v>
@@ -5664,86 +5778,86 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>19</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>19</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5751,27 +5865,27 @@
         <v>13</v>
       </c>
       <c r="B8" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="0" t="s">
         <v>94</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5779,13 +5893,27 @@
         <v>17</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="C10" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="0" t="s">
-        <v>90</v>
+      <c r="B11" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -5804,10 +5932,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5822,69 +5950,69 @@
         <v>0</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5892,13 +6020,13 @@
         <v>12</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5906,13 +6034,27 @@
         <v>12</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>114</v>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>